<commit_message>
tring to recreate no. of samples graph. FINALLY FIXED MCMC!! :D
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/jamie_watts_stfc_ac_uk/Documents/Documents/python/git_projects/THz-Compressed-Sensing/compressed_sensing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/jamie_watts_stfc_ac_uk/Documents/Documents/python/git_projects/THz-Compressed-Sensing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="405" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABB5EB79-459B-4376-83B9-D950F529FA46}"/>
+  <xr:revisionPtr revIDLastSave="442" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0E6D178-17F2-4EFB-92AB-E82A3B460B10}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="2430" windowWidth="28725" windowHeight="10530" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1D OLD" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="63">
   <si>
     <t>1dmock.csv (old format)</t>
   </si>
@@ -170,9 +170,6 @@
     <t>1dmockanderrors12.csv</t>
   </si>
   <si>
-    <t>1dmockanderrors13</t>
-  </si>
-  <si>
     <t>training_set/</t>
   </si>
   <si>
@@ -194,25 +191,43 @@
     <t>number of interferograms</t>
   </si>
   <si>
-    <t>1dmockanderrors14</t>
-  </si>
-  <si>
     <t>Brute force solved for 4 detectors.</t>
   </si>
   <si>
     <t>Seems to follow noiseless solution</t>
   </si>
   <si>
-    <t>1dmockanderrors15</t>
-  </si>
-  <si>
-    <t>1dmockanderrors16</t>
-  </si>
-  <si>
     <t>training_set4</t>
   </si>
   <si>
     <t>0.2-5</t>
+  </si>
+  <si>
+    <t>training_set5</t>
+  </si>
+  <si>
+    <t>2.0-4.0</t>
+  </si>
+  <si>
+    <t>0.5-2</t>
+  </si>
+  <si>
+    <t>1dmockanderrors13.csv</t>
+  </si>
+  <si>
+    <t>1dmockanderrors14.csv</t>
+  </si>
+  <si>
+    <t>1dmockanderrors15.csv</t>
+  </si>
+  <si>
+    <t>1dmockanderrors16.csv</t>
+  </si>
+  <si>
+    <t>1dmockanderrors17.csv</t>
+  </si>
+  <si>
+    <t>Noisey version of 15</t>
   </si>
 </sst>
 </file>
@@ -256,12 +271,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -303,8 +319,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}" name="Table43" displayName="Table43" ref="B3:M19" totalsRowShown="0">
-  <autoFilter ref="B3:M19" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}" name="Table43" displayName="Table43" ref="B3:M20" totalsRowShown="0">
+  <autoFilter ref="B3:M20" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{27BB0DD3-D6F3-4A85-9E2D-A2D5E808B35F}" name="name"/>
     <tableColumn id="2" xr3:uid="{4BDE5EDC-72BC-487E-A973-D9B010515F48}" name="array length (pixels)"/>
@@ -635,15 +651,15 @@
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -843,28 +859,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35A9735-8756-4052-9A25-A87B0D23F6C4}">
-  <dimension ref="B2:M19"/>
+  <dimension ref="B2:M20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -1319,7 +1338,7 @@
         <v>30</v>
       </c>
       <c r="M14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
@@ -1357,12 +1376,12 @@
         <v>30</v>
       </c>
       <c r="M15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C16">
         <v>200</v>
@@ -1397,7 +1416,7 @@
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C17">
         <v>100</v>
@@ -1432,7 +1451,7 @@
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C18">
         <v>200</v>
@@ -1465,12 +1484,12 @@
         <v>30</v>
       </c>
       <c r="M18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C19">
         <v>200</v>
@@ -1503,7 +1522,45 @@
         <v>30</v>
       </c>
       <c r="M19" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20">
+        <v>200</v>
+      </c>
+      <c r="D20">
+        <v>200</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>1.5</v>
+      </c>
+      <c r="G20">
+        <v>60</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>20</v>
+      </c>
+      <c r="L20">
+        <v>30</v>
+      </c>
+      <c r="M20" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1519,10 +1576,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D7BFC62-FF4F-4DA1-97AB-A53A0749BD39}">
-  <dimension ref="B2:L7"/>
+  <dimension ref="B2:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1537,17 +1594,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
@@ -1579,7 +1636,7 @@
         <v>16</v>
       </c>
       <c r="K3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L3" t="s">
         <v>20</v>
@@ -1587,7 +1644,7 @@
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4">
         <v>200</v>
@@ -1596,10 +1653,10 @@
         <v>200</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G4">
         <v>60</v>
@@ -1619,7 +1676,7 @@
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5">
         <v>200</v>
@@ -1628,10 +1685,10 @@
         <v>200</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G5">
         <v>60</v>
@@ -1651,7 +1708,7 @@
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -1660,10 +1717,10 @@
         <v>400</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G6">
         <v>60</v>
@@ -1683,7 +1740,7 @@
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C7">
         <v>200</v>
@@ -1692,10 +1749,10 @@
         <v>200</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G7">
         <v>60</v>
@@ -1711,6 +1768,38 @@
       </c>
       <c r="K7">
         <v>2500</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8">
+        <v>200</v>
+      </c>
+      <c r="D8">
+        <v>200</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8">
+        <v>60</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>20</v>
+      </c>
+      <c r="J8">
+        <v>30</v>
+      </c>
+      <c r="K8">
+        <v>900</v>
       </c>
     </row>
   </sheetData>
@@ -1735,18 +1824,18 @@
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">

</xml_diff>

<commit_message>
making graphs for report
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/jamie_watts_stfc_ac_uk/Documents/Documents/python/git_projects/THz-Compressed-Sensing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="442" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0E6D178-17F2-4EFB-92AB-E82A3B460B10}"/>
+  <xr:revisionPtr revIDLastSave="447" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4C4EE97-28D7-4262-A814-0CB1900DB95F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8700" yWindow="4095" windowWidth="19110" windowHeight="10530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1D OLD" sheetId="1" r:id="rId1"/>
@@ -861,13 +861,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35A9735-8756-4052-9A25-A87B0D23F6C4}">
   <dimension ref="B2:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
reverted block-based CS. created LS vs CS interferogram
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/jamie_watts_stfc_ac_uk/Documents/Documents/python/git_projects/THz-Compressed-Sensing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="447" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4C4EE97-28D7-4262-A814-0CB1900DB95F}"/>
+  <xr:revisionPtr revIDLastSave="458" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CEAA7BB1-08B5-47D5-9694-09820D9CFFDC}"/>
   <bookViews>
-    <workbookView xWindow="8700" yWindow="4095" windowWidth="19110" windowHeight="10530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1935" yWindow="3390" windowWidth="19110" windowHeight="10530" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1D OLD" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
   <si>
     <t>1dmock.csv (old format)</t>
   </si>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>Noisey version of 15</t>
+  </si>
+  <si>
+    <t>2dmock1.fits/.csv</t>
   </si>
 </sst>
 </file>
@@ -861,7 +864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35A9735-8756-4052-9A25-A87B0D23F6C4}">
   <dimension ref="B2:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+    <sheetView topLeftCell="B10" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1820,10 +1823,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEC75F5B-FD8B-46F1-B910-69CAC90BFB37}">
-  <dimension ref="B2:L4"/>
+  <dimension ref="B2:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1906,6 +1909,38 @@
         <v>10</v>
       </c>
       <c r="K4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5">
+        <v>75</v>
+      </c>
+      <c r="E5">
+        <v>200</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>30</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>20</v>
+      </c>
+      <c r="K5">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Everything sucks. Need to somehow get results for experimental source.
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/jamie_watts_stfc_ac_uk/Documents/Documents/python/git_projects/THz-Compressed-Sensing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="458" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CEAA7BB1-08B5-47D5-9694-09820D9CFFDC}"/>
+  <xr:revisionPtr revIDLastSave="459" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D083474-A54F-4A4E-9D3A-E90C14DFE842}"/>
   <bookViews>
     <workbookView xWindow="1935" yWindow="3390" windowWidth="19110" windowHeight="10530" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1826,7 +1826,7 @@
   <dimension ref="B2:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1938,7 +1938,7 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="K5">
         <v>30</v>

</xml_diff>

<commit_message>
made new mock interferograms to 'predict' experiment
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/jamie_watts_stfc_ac_uk/Documents/Documents/python/git_projects/THz-Compressed-Sensing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="459" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D083474-A54F-4A4E-9D3A-E90C14DFE842}"/>
+  <xr:revisionPtr revIDLastSave="480" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FCCEC2B-BBE0-42D0-9928-E4739C4BC22F}"/>
   <bookViews>
-    <workbookView xWindow="1935" yWindow="3390" windowWidth="19110" windowHeight="10530" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7905" yWindow="3795" windowWidth="19110" windowHeight="10530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1D OLD" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="70">
   <si>
     <t>1dmock.csv (old format)</t>
   </si>
@@ -231,6 +231,24 @@
   </si>
   <si>
     <t>2dmock1.fits/.csv</t>
+  </si>
+  <si>
+    <t>1dmockanderrors18.csv</t>
+  </si>
+  <si>
+    <t>[Two equal peaks at 0.27 and 0.45]</t>
+  </si>
+  <si>
+    <t>[modulated by a gaussian with FWHM = 35mm]</t>
+  </si>
+  <si>
+    <t>1dmockanderrors19.csv</t>
+  </si>
+  <si>
+    <t>1dmockanderrors20.csv</t>
+  </si>
+  <si>
+    <t>1dmockanderrors21.csv</t>
   </si>
 </sst>
 </file>
@@ -322,8 +340,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}" name="Table43" displayName="Table43" ref="B3:M20" totalsRowShown="0">
-  <autoFilter ref="B3:M20" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}" name="Table43" displayName="Table43" ref="B3:M24" totalsRowShown="0">
+  <autoFilter ref="B3:M24" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{27BB0DD3-D6F3-4A85-9E2D-A2D5E808B35F}" name="name"/>
     <tableColumn id="2" xr3:uid="{4BDE5EDC-72BC-487E-A973-D9B010515F48}" name="array length (pixels)"/>
@@ -862,10 +880,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35A9735-8756-4052-9A25-A87B0D23F6C4}">
-  <dimension ref="B2:M20"/>
+  <dimension ref="B2:M24"/>
   <sheetViews>
-    <sheetView topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1569,6 +1587,146 @@
       </c>
       <c r="M20" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21">
+        <v>53</v>
+      </c>
+      <c r="D21">
+        <v>1000</v>
+      </c>
+      <c r="E21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" t="s">
+        <v>66</v>
+      </c>
+      <c r="G21">
+        <v>200</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>20</v>
+      </c>
+      <c r="L21">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22">
+        <v>53</v>
+      </c>
+      <c r="D22">
+        <v>1000</v>
+      </c>
+      <c r="E22" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22">
+        <v>200</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23">
+        <v>53</v>
+      </c>
+      <c r="D23">
+        <v>1000</v>
+      </c>
+      <c r="E23">
+        <v>0.27</v>
+      </c>
+      <c r="F23" t="s">
+        <v>66</v>
+      </c>
+      <c r="G23">
+        <v>200</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>20</v>
+      </c>
+      <c r="L23">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24">
+        <v>53</v>
+      </c>
+      <c r="D24">
+        <v>1000</v>
+      </c>
+      <c r="E24">
+        <v>0.27</v>
+      </c>
+      <c r="F24" t="s">
+        <v>66</v>
+      </c>
+      <c r="G24">
+        <v>200</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1825,7 +1983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEC75F5B-FD8B-46F1-B910-69CAC90BFB37}">
   <dimension ref="B2:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
CS is able to resolve second experimental peak based on simulated interferogram!
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/jamie_watts_stfc_ac_uk/Documents/Documents/python/git_projects/THz-Compressed-Sensing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="480" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3FCCEC2B-BBE0-42D0-9928-E4739C4BC22F}"/>
+  <xr:revisionPtr revIDLastSave="494" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{019D772E-E182-423D-A02B-5C802D0C5F40}"/>
   <bookViews>
-    <workbookView xWindow="7905" yWindow="3795" windowWidth="19110" windowHeight="10530" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7905" yWindow="3795" windowWidth="19110" windowHeight="10530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1D OLD" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="72">
   <si>
     <t>1dmock.csv (old format)</t>
   </si>
@@ -249,6 +249,12 @@
   </si>
   <si>
     <t>1dmockanderrors21.csv</t>
+  </si>
+  <si>
+    <t>1dmockanderrors22.csv</t>
+  </si>
+  <si>
+    <t>[Two equal peaks at 0.27 and 0.42]</t>
   </si>
 </sst>
 </file>
@@ -340,8 +346,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}" name="Table43" displayName="Table43" ref="B3:M24" totalsRowShown="0">
-  <autoFilter ref="B3:M24" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}" name="Table43" displayName="Table43" ref="B3:M25" totalsRowShown="0">
+  <autoFilter ref="B3:M25" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{27BB0DD3-D6F3-4A85-9E2D-A2D5E808B35F}" name="name"/>
     <tableColumn id="2" xr3:uid="{4BDE5EDC-72BC-487E-A973-D9B010515F48}" name="array length (pixels)"/>
@@ -665,7 +671,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -880,10 +886,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35A9735-8756-4052-9A25-A87B0D23F6C4}">
-  <dimension ref="B2:M24"/>
+  <dimension ref="B2:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1726,6 +1732,41 @@
         <v>0</v>
       </c>
       <c r="L24">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25">
+        <v>53</v>
+      </c>
+      <c r="D25">
+        <v>1000</v>
+      </c>
+      <c r="E25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" t="s">
+        <v>66</v>
+      </c>
+      <c r="G25">
+        <v>200</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
re-made optimisation method comparason graph with new simulated interferograms
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/jamie_watts_stfc_ac_uk/Documents/Documents/python/git_projects/THz-Compressed-Sensing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcr73298\Documents\THz-Compressed-Sensing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="494" documentId="11_F25DC773A252ABDACC104822511E71405BDE58F8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{019D772E-E182-423D-A02B-5C802D0C5F40}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1430B03-F1AF-415D-B6AA-7EF75D56791C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7905" yWindow="3795" windowWidth="19110" windowHeight="10530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1D OLD" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="78">
   <si>
     <t>1dmock.csv (old format)</t>
   </si>
@@ -255,6 +255,24 @@
   </si>
   <si>
     <t>[Two equal peaks at 0.27 and 0.42]</t>
+  </si>
+  <si>
+    <t>1dmockanderrors23.csv</t>
+  </si>
+  <si>
+    <t>we're so back</t>
+  </si>
+  <si>
+    <t>same but with more noise</t>
+  </si>
+  <si>
+    <t>1dmockanderrors24.csv</t>
+  </si>
+  <si>
+    <t>1dmockanderrors25.csv</t>
+  </si>
+  <si>
+    <t>same but with larger FWHM</t>
   </si>
 </sst>
 </file>
@@ -325,10 +343,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{70A695AD-CD1A-4939-8512-07C2F4E67915}" name="Table3" displayName="Table3" ref="B2:H9" totalsRowShown="0">
   <autoFilter ref="B2:H9" xr:uid="{70A695AD-CD1A-4939-8512-07C2F4E67915}"/>
@@ -346,8 +360,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}" name="Table43" displayName="Table43" ref="B3:M25" totalsRowShown="0">
-  <autoFilter ref="B3:M25" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}" name="Table43" displayName="Table43" ref="B3:M28" totalsRowShown="0">
+  <autoFilter ref="B3:M28" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{27BB0DD3-D6F3-4A85-9E2D-A2D5E808B35F}" name="name"/>
     <tableColumn id="2" xr3:uid="{4BDE5EDC-72BC-487E-A973-D9B010515F48}" name="array length (pixels)"/>
@@ -671,7 +685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -886,10 +900,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35A9735-8756-4052-9A25-A87B0D23F6C4}">
-  <dimension ref="B2:M25"/>
+  <dimension ref="B2:M28"/>
   <sheetViews>
-    <sheetView topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1768,6 +1782,120 @@
       </c>
       <c r="L25">
         <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26">
+        <v>53</v>
+      </c>
+      <c r="D26">
+        <v>1000</v>
+      </c>
+      <c r="E26">
+        <v>0.27</v>
+      </c>
+      <c r="F26">
+        <v>0.05</v>
+      </c>
+      <c r="G26">
+        <v>200</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>5</v>
+      </c>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27">
+        <v>53</v>
+      </c>
+      <c r="D27">
+        <v>1000</v>
+      </c>
+      <c r="E27">
+        <v>0.27</v>
+      </c>
+      <c r="F27">
+        <v>0.05</v>
+      </c>
+      <c r="G27">
+        <v>200</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>10</v>
+      </c>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28">
+        <v>53</v>
+      </c>
+      <c r="D28">
+        <v>1000</v>
+      </c>
+      <c r="E28">
+        <v>0.27</v>
+      </c>
+      <c r="F28">
+        <v>0.1</v>
+      </c>
+      <c r="G28">
+        <v>200</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>5</v>
+      </c>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
investigated rip and updated histogram graph
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcr73298\Documents\THz-Compressed-Sensing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36454504-C015-4006-B73D-72D47D4714EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4CB470-791F-4D56-9F84-FE7AEA35FCE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="82">
   <si>
     <t>1dmock.csv (old format)</t>
   </si>
@@ -273,6 +273,18 @@
   </si>
   <si>
     <t>same but with larger FWHM</t>
+  </si>
+  <si>
+    <t>1dmockanderrors26.csv</t>
+  </si>
+  <si>
+    <t>same but with higher central frequency</t>
+  </si>
+  <si>
+    <t>1dmockanderrors27.csv</t>
+  </si>
+  <si>
+    <t>noiseless version of 26</t>
   </si>
 </sst>
 </file>
@@ -360,8 +372,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}" name="Table43" displayName="Table43" ref="B3:M28" totalsRowShown="0">
-  <autoFilter ref="B3:M28" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}" name="Table43" displayName="Table43" ref="B3:M30" totalsRowShown="0">
+  <autoFilter ref="B3:M30" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{27BB0DD3-D6F3-4A85-9E2D-A2D5E808B35F}" name="name"/>
     <tableColumn id="2" xr3:uid="{4BDE5EDC-72BC-487E-A973-D9B010515F48}" name="array length (pixels)"/>
@@ -900,10 +912,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35A9735-8756-4052-9A25-A87B0D23F6C4}">
-  <dimension ref="B2:M28"/>
+  <dimension ref="B2:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1896,6 +1908,82 @@
       </c>
       <c r="M28" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29">
+        <v>53</v>
+      </c>
+      <c r="D29">
+        <v>1000</v>
+      </c>
+      <c r="E29">
+        <v>0.3</v>
+      </c>
+      <c r="F29">
+        <v>0.1</v>
+      </c>
+      <c r="G29">
+        <v>200</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>5</v>
+      </c>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30">
+        <v>53</v>
+      </c>
+      <c r="D30">
+        <v>1000</v>
+      </c>
+      <c r="E30">
+        <v>0.3</v>
+      </c>
+      <c r="F30">
+        <v>0.1</v>
+      </c>
+      <c r="G30">
+        <v>200</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <v>1</v>
+      </c>
+      <c r="M30" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
realised that the peaks are 270 and 180GHz. Updating graphs for new experimental findings.
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcr73298\Documents\THz-Compressed-Sensing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/jamie_watts1_stfc_ac_uk/Documents/Documents/THz-Compressed-Sensing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4CB470-791F-4D56-9F84-FE7AEA35FCE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{2A4CB470-791F-4D56-9F84-FE7AEA35FCE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE02AFDC-3508-499E-A220-2A7CBD4797ED}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1D OLD" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="88">
   <si>
     <t>1dmock.csv (old format)</t>
   </si>
@@ -285,6 +285,24 @@
   </si>
   <si>
     <t>noiseless version of 26</t>
+  </si>
+  <si>
+    <t>1dmockanderrors28.csv</t>
+  </si>
+  <si>
+    <t>1dmockanderrors29.csv</t>
+  </si>
+  <si>
+    <t>noiseless</t>
+  </si>
+  <si>
+    <t>1dmockanderrors30.csv</t>
+  </si>
+  <si>
+    <t>[Two equal peaks at 0.182 and 0.273]</t>
+  </si>
+  <si>
+    <t>realistic interferogram, very simular to what was observed</t>
   </si>
 </sst>
 </file>
@@ -328,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -338,6 +356,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,8 +391,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}" name="Table43" displayName="Table43" ref="B3:M30" totalsRowShown="0">
-  <autoFilter ref="B3:M30" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}" name="Table43" displayName="Table43" ref="B3:M33" totalsRowShown="0">
+  <autoFilter ref="B3:M33" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{27BB0DD3-D6F3-4A85-9E2D-A2D5E808B35F}" name="name"/>
     <tableColumn id="2" xr3:uid="{4BDE5EDC-72BC-487E-A973-D9B010515F48}" name="array length (pixels)"/>
@@ -912,10 +931,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35A9735-8756-4052-9A25-A87B0D23F6C4}">
-  <dimension ref="B2:M30"/>
+  <dimension ref="B2:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1984,6 +2003,117 @@
       </c>
       <c r="M30" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31">
+        <v>99</v>
+      </c>
+      <c r="D31">
+        <v>500</v>
+      </c>
+      <c r="E31">
+        <v>0.3</v>
+      </c>
+      <c r="F31">
+        <v>0.05</v>
+      </c>
+      <c r="G31">
+        <v>360</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>5</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32">
+        <v>99</v>
+      </c>
+      <c r="D32">
+        <v>500</v>
+      </c>
+      <c r="E32">
+        <v>0.3</v>
+      </c>
+      <c r="F32">
+        <v>0.05</v>
+      </c>
+      <c r="G32">
+        <v>360</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33">
+        <v>99</v>
+      </c>
+      <c r="D33">
+        <v>500</v>
+      </c>
+      <c r="E33" t="s">
+        <v>86</v>
+      </c>
+      <c r="F33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G33">
+        <v>360</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>1</v>
+      </c>
+      <c r="M33" s="5" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated graphs but data is too noisy. 0.5 pixel pitch might be too ambitious.
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/jamie_watts1_stfc_ac_uk/Documents/Documents/THz-Compressed-Sensing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{2A4CB470-791F-4D56-9F84-FE7AEA35FCE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE02AFDC-3508-499E-A220-2A7CBD4797ED}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{2A4CB470-791F-4D56-9F84-FE7AEA35FCE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{004EF972-61B9-4DA6-95B9-A451C7B171D5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -934,7 +934,7 @@
   <dimension ref="B2:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2019,7 +2019,7 @@
         <v>0.3</v>
       </c>
       <c r="F31">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="G31">
         <v>360</v>
@@ -2054,7 +2054,7 @@
         <v>0.3</v>
       </c>
       <c r="F32">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="G32">
         <v>360</v>

</xml_diff>

<commit_message>
continueing to update graphs for new experimental data. I now have a good results graph.
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/jamie_watts1_stfc_ac_uk/Documents/Documents/THz-Compressed-Sensing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{2A4CB470-791F-4D56-9F84-FE7AEA35FCE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{004EF972-61B9-4DA6-95B9-A451C7B171D5}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{2A4CB470-791F-4D56-9F84-FE7AEA35FCE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13F78C31-8517-412F-9CCC-D11569EA116A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1D OLD" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="93">
   <si>
     <t>1dmock.csv (old format)</t>
   </si>
@@ -303,6 +303,21 @@
   </si>
   <si>
     <t>realistic interferogram, very simular to what was observed</t>
+  </si>
+  <si>
+    <t>1dmockanderrors31.csv</t>
+  </si>
+  <si>
+    <t>1dmockanderrors32.csv</t>
+  </si>
+  <si>
+    <t>1dmockanderrors33.csv</t>
+  </si>
+  <si>
+    <t>realistic but larger pixel pitch</t>
+  </si>
+  <si>
+    <t>[modulated by a gaussian with FWHM = 30mm]</t>
   </si>
 </sst>
 </file>
@@ -391,8 +406,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}" name="Table43" displayName="Table43" ref="B3:M33" totalsRowShown="0">
-  <autoFilter ref="B3:M33" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}" name="Table43" displayName="Table43" ref="B3:M36" totalsRowShown="0">
+  <autoFilter ref="B3:M36" xr:uid="{D61E1BB3-3866-446A-837F-87249BC61D4A}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{27BB0DD3-D6F3-4A85-9E2D-A2D5E808B35F}" name="name"/>
     <tableColumn id="2" xr3:uid="{4BDE5EDC-72BC-487E-A973-D9B010515F48}" name="array length (pixels)"/>
@@ -931,10 +946,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35A9735-8756-4052-9A25-A87B0D23F6C4}">
-  <dimension ref="B2:M33"/>
+  <dimension ref="B2:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2114,6 +2129,117 @@
       </c>
       <c r="M33" s="5" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34">
+        <v>50</v>
+      </c>
+      <c r="D34">
+        <v>1000</v>
+      </c>
+      <c r="E34">
+        <v>0.3</v>
+      </c>
+      <c r="F34">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G34">
+        <v>360</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>5</v>
+      </c>
+      <c r="L34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35">
+        <v>50</v>
+      </c>
+      <c r="D35">
+        <v>1000</v>
+      </c>
+      <c r="E35">
+        <v>0.3</v>
+      </c>
+      <c r="F35">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G35">
+        <v>360</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>1</v>
+      </c>
+      <c r="M35" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36">
+        <v>50</v>
+      </c>
+      <c r="D36">
+        <v>1000</v>
+      </c>
+      <c r="E36" t="s">
+        <v>86</v>
+      </c>
+      <c r="F36" t="s">
+        <v>92</v>
+      </c>
+      <c r="G36">
+        <v>366</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+      <c r="M36" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all graphs updated :)
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stfc365-my.sharepoint.com/personal/jamie_watts1_stfc_ac_uk/Documents/Documents/THz-Compressed-Sensing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{2A4CB470-791F-4D56-9F84-FE7AEA35FCE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13F78C31-8517-412F-9CCC-D11569EA116A}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{2A4CB470-791F-4D56-9F84-FE7AEA35FCE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62DF0A00-86C7-46D0-B538-A86A0A216D02}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -948,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35A9735-8756-4052-9A25-A87B0D23F6C4}">
   <dimension ref="B2:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2107,10 +2107,10 @@
         <v>86</v>
       </c>
       <c r="F33" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="G33">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="H33">
         <v>1</v>

</xml_diff>

<commit_message>
re-running for L2 error. alpha = 1e-2 seems to work well. Theory reccomends 5e-2.
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -368,10 +368,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,6 +387,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -738,15 +742,15 @@
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -949,7 +953,7 @@
   <dimension ref="B2:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,19 +967,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -2127,7 +2131,7 @@
       <c r="L33">
         <v>1</v>
       </c>
-      <c r="M33" s="5" t="s">
+      <c r="M33" s="4" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2273,17 +2277,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
@@ -2503,18 +2507,18 @@
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">

</xml_diff>